<commit_message>
Excluding PHH and OTH for all EAC countries (not Just Kenia) and doing extimation with 3 different transformation of the independent variables.
</commit_message>
<xml_diff>
--- a/Tables/GROWTH_EST_MAN_TFE.xlsx
+++ b/Tables/GROWTH_EST_MAN_TFE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -53,6 +53,9 @@
     <t xml:space="preserve">R2 Within</t>
   </si>
   <si>
+    <t xml:space="preserve">Std. Errors</t>
+  </si>
+  <si>
     <t xml:space="preserve">FE: cs</t>
   </si>
   <si>
@@ -62,10 +65,7 @@
     <t xml:space="preserve">FE: sy</t>
   </si>
   <si>
-    <t xml:space="preserve">Std. errors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* p &lt; 0.1, ** p &lt; 0.05, *** p &lt; 0.01</t>
+    <t xml:space="preserve">+ p &lt; 0.1, * p &lt; 0.05, ** p &lt; 0.01, *** p &lt; 0.001</t>
   </si>
   <si>
     <t xml:space="preserve">FD</t>
@@ -74,193 +74,292 @@
     <t xml:space="preserve">0.0678***</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.0096)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.4875***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.3312)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.9133**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.3705)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.3446)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.9897***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.5550)</t>
+    <t xml:space="preserve">(0.0088)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.4875*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.5558)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.5808)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5380*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.2403)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.9897*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1.4786)</t>
   </si>
   <si>
     <t xml:space="preserve">2.4464***</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.5447)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.4672)</t>
+    <t xml:space="preserve">(0.4453)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.2851)</t>
   </si>
   <si>
     <t xml:space="preserve">Clustered (cs)</t>
   </si>
   <si>
-    <t xml:space="preserve">FD-TFE</t>
+    <t xml:space="preserve">FD-FE</t>
   </si>
   <si>
     <t xml:space="preserve">-5.5255**</t>
   </si>
   <si>
-    <t xml:space="preserve">(2.1489)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3.9961)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.7522)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.4871)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.3725)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.3174)</t>
+    <t xml:space="preserve">(1.8918)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(3.3684)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1.6251)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.4625)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.4383)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.3696)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three-way (cs &amp; cy &amp; sy)</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">Three-way (cs &amp; cy &amp; sy)</t>
-  </si>
-  <si>
     <t xml:space="preserve">FE</t>
   </si>
   <si>
-    <t xml:space="preserve">-5.9522***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.8947)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5.2555)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4.1243)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.9184)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.0540)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.5748)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FD Elas</t>
+    <t xml:space="preserve">-5.9522*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2.4494)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5.6843)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4.2572)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1.0006)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.9402)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.5726)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD ES</t>
   </si>
   <si>
     <t xml:space="preserve">0.0752***</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.0050)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1546***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0533)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1360**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0594)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1782***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0551)</t>
+    <t xml:space="preserve">(0.0038)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1546+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0901)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1360***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0337)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1782**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0506)</t>
   </si>
   <si>
     <t xml:space="preserve">0.9845***</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.0303)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2056***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0384)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0328)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FD-TFE Elas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.8395***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.2720)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.2382)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.2443)</t>
+    <t xml:space="preserve">(0.0505)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2056*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0771)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD-FE ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.8395**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.2898)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.3627*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.1647)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.2602)</t>
   </si>
   <si>
     <t xml:space="preserve">0.8140***</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.0669)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0490)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0203)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FE Elas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.6364**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.3142)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.6820**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.2648)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.2528)</t>
+    <t xml:space="preserve">(0.0867)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0519)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0230)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.6364*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.2812)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.6820***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.1900)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4091+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.2211)</t>
   </si>
   <si>
     <t xml:space="preserve">0.8362***</t>
   </si>
   <si>
-    <t xml:space="preserve">(0.0465)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0652)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.0941)</t>
+    <t xml:space="preserve">(0.0643)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0837)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0908)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0419***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0041)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.5477***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0491)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0942+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0466)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0590*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0252)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8882***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0470)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1228*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0455)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0197)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD-FE E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.4025***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0599)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0388)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0249)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9013***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0281)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FE E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.3972***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0954)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0986+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0567)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1184*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0568)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8926***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0478)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0838)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.0894)</t>
   </si>
 </sst>
 </file>
@@ -672,6 +771,9 @@
     <col min="5" max="5" width="10.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="10.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="10.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="10.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="10.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="10.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="NA" customHeight="1">
@@ -691,10 +793,19 @@
         <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="2" ht="NA" customHeight="1">
@@ -719,6 +830,15 @@
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" ht="NA" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -740,6 +860,15 @@
         <v>2</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -760,11 +889,20 @@
         <v>53</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="5" ht="NA" customHeight="1">
       <c r="A5" s="3" t="s">
@@ -783,18 +921,27 @@
         <v>54</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>75</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" ht="NA" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
+      <c r="B6" s="3" t="n">
+        <v>-0.9133</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>-3.2163</v>
@@ -805,19 +952,28 @@
       <c r="E6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="3" t="n">
-        <v>-0.3627</v>
+      <c r="F6" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>-0.0548</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="7" ht="NA" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>35</v>
@@ -833,14 +989,23 @@
       </c>
       <c r="G7" s="3" t="s">
         <v>77</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="8" ht="NA" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="n">
-        <v>0.538</v>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>2.4802</v>
@@ -854,8 +1019,17 @@
       <c r="F8" s="3" t="n">
         <v>0.3872</v>
       </c>
-      <c r="G8" s="3" t="n">
-        <v>0.4091</v>
+      <c r="G8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>0.0175</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -878,7 +1052,16 @@
         <v>68</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
@@ -901,7 +1084,16 @@
         <v>69</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" ht="NA" customHeight="1">
@@ -924,7 +1116,16 @@
         <v>70</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" ht="NA" customHeight="1">
@@ -949,6 +1150,15 @@
       <c r="G12" s="3" t="n">
         <v>0.1013</v>
       </c>
+      <c r="H12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>0.0183</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>0.0883</v>
+      </c>
     </row>
     <row r="13" ht="NA" customHeight="1">
       <c r="A13" s="3" t="s">
@@ -970,7 +1180,16 @@
         <v>71</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="14" ht="NA" customHeight="1">
@@ -995,6 +1214,15 @@
       <c r="G14" s="3" t="n">
         <v>-0.1399</v>
       </c>
+      <c r="H14" s="3" t="n">
+        <v>-0.0097</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>0.0252</v>
+      </c>
+      <c r="J14" s="3" t="n">
+        <v>-0.1072</v>
+      </c>
     </row>
     <row r="15" ht="NA" customHeight="1">
       <c r="A15" s="4" t="s">
@@ -1010,13 +1238,22 @@
         <v>49</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>72</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="16" ht="NA" customHeight="1">
@@ -1041,6 +1278,15 @@
       <c r="G16" s="2" t="n">
         <v>360</v>
       </c>
+      <c r="H16" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="17" ht="NA" customHeight="1">
       <c r="A17" s="3" t="s">
@@ -1064,6 +1310,15 @@
       <c r="G17" s="3" t="n">
         <v>0.999</v>
       </c>
+      <c r="H17" s="3" t="n">
+        <v>0.849</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" ht="NA" customHeight="1">
       <c r="A18" s="3" t="s">
@@ -1087,6 +1342,15 @@
       <c r="G18" s="3" t="n">
         <v>0.999</v>
       </c>
+      <c r="H18" s="3" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>0.981</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>0.999</v>
+      </c>
     </row>
     <row r="19" ht="NA" customHeight="1">
       <c r="A19" s="3" t="s">
@@ -1110,27 +1374,45 @@
       <c r="G19" s="3" t="n">
         <v>0.925</v>
       </c>
+      <c r="H19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>0.936</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>0.94</v>
+      </c>
     </row>
     <row r="20" ht="NA" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="G20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1142,19 +1424,28 @@
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" ht="NA" customHeight="1">
@@ -1165,19 +1456,28 @@
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" ht="NA" customHeight="1">
@@ -1185,7 +1485,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>41</v>
@@ -1194,7 +1494,7 @@
         <v>41</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>41</v>
@@ -1202,33 +1502,51 @@
       <c r="G23" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="H23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="24" ht="NA" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>